<commit_message>
Update with latest invivoPKfits
</commit_message>
<xml_diff>
--- a/SupTable-QSPRPredsandInVitroData.xlsx
+++ b/SupTable-QSPRPredsandInVitroData.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\tkqsars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B521052F-9E3F-4E9C-8FC4-518DEB75084B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF4D1CB-B5FF-4CCC-BA5C-059208889628}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="1050" windowWidth="20460" windowHeight="11490"/>
+    <workbookView xWindow="8415" yWindow="3675" windowWidth="20265" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SupTable-QSPRPredsandInVitroDat" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="325">
   <si>
     <t>DTXSID</t>
   </si>
@@ -1000,7 +1000,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1478,9 +1478,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -1836,11 +1835,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="L97" sqref="A1:U102"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:U102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1852,7 +1851,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -1917,7 +1916,7 @@
       <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>23</v>
       </c>
       <c r="D2">
@@ -1926,7 +1925,7 @@
       <c r="E2">
         <v>380</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>2.2600000000000001E-11</v>
       </c>
       <c r="G2">
@@ -1938,7 +1937,7 @@
       <c r="I2">
         <v>150</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="1">
         <v>1.2700000000000001E-7</v>
       </c>
       <c r="K2">
@@ -1947,8 +1946,8 @@
       <c r="L2">
         <v>8.59</v>
       </c>
-      <c r="M2">
-        <v>0</v>
+      <c r="M2" t="s">
+        <v>24</v>
       </c>
       <c r="N2">
         <v>1090</v>
@@ -1982,7 +1981,7 @@
       <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>27</v>
       </c>
       <c r="D3">
@@ -1991,7 +1990,7 @@
       <c r="E3">
         <v>300</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>2.9600000000000001E-9</v>
       </c>
       <c r="G3">
@@ -2003,7 +2002,7 @@
       <c r="I3">
         <v>141</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>2.8900000000000001E-7</v>
       </c>
       <c r="K3">
@@ -2025,7 +2024,7 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>0.05</v>
+        <v>6.3799999999999996E-2</v>
       </c>
       <c r="R3">
         <v>5.36</v>
@@ -2047,7 +2046,7 @@
       <c r="B4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>30</v>
       </c>
       <c r="D4">
@@ -2056,7 +2055,7 @@
       <c r="E4">
         <v>327</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>5.7200000000000001E-9</v>
       </c>
       <c r="G4">
@@ -2068,7 +2067,7 @@
       <c r="I4">
         <v>62.1</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>9.3300000000000005E-6</v>
       </c>
       <c r="K4">
@@ -2090,7 +2089,7 @@
         <v>21.7</v>
       </c>
       <c r="Q4">
-        <v>4.1500000000000002E-2</v>
+        <v>4.1599999999999998E-2</v>
       </c>
       <c r="R4">
         <v>16.600000000000001</v>
@@ -2112,7 +2111,7 @@
       <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>33</v>
       </c>
       <c r="D5">
@@ -2157,8 +2156,8 @@
       <c r="Q5" t="s">
         <v>24</v>
       </c>
-      <c r="R5">
-        <v>8.82</v>
+      <c r="R5" t="s">
+        <v>24</v>
       </c>
       <c r="S5" t="s">
         <v>24</v>
@@ -2177,7 +2176,7 @@
       <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>36</v>
       </c>
       <c r="D6">
@@ -2186,7 +2185,7 @@
       <c r="E6">
         <v>404</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>1.8500000000000001E-10</v>
       </c>
       <c r="G6">
@@ -2198,7 +2197,7 @@
       <c r="I6">
         <v>262</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="1">
         <v>2.0299999999999998E-9</v>
       </c>
       <c r="K6">
@@ -2220,7 +2219,7 @@
         <v>6.25</v>
       </c>
       <c r="Q6">
-        <v>3.9199999999999999E-2</v>
+        <v>4.0599999999999997E-2</v>
       </c>
       <c r="R6">
         <v>27.8</v>
@@ -2242,7 +2241,7 @@
       <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>39</v>
       </c>
       <c r="D7">
@@ -2287,8 +2286,8 @@
       <c r="Q7" t="s">
         <v>24</v>
       </c>
-      <c r="R7">
-        <v>8.82</v>
+      <c r="R7" t="s">
+        <v>24</v>
       </c>
       <c r="S7" t="s">
         <v>24</v>
@@ -2307,7 +2306,7 @@
       <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>42</v>
       </c>
       <c r="D8">
@@ -2316,7 +2315,7 @@
       <c r="E8">
         <v>305</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>7.1299999999999999E-7</v>
       </c>
       <c r="G8">
@@ -2350,10 +2349,10 @@
         <v>21.7</v>
       </c>
       <c r="Q8">
-        <v>5.7099999999999998E-2</v>
-      </c>
-      <c r="R8">
-        <v>10.4</v>
+        <v>6.2300000000000001E-2</v>
+      </c>
+      <c r="R8" t="s">
+        <v>24</v>
       </c>
       <c r="S8" t="s">
         <v>24</v>
@@ -2372,7 +2371,7 @@
       <c r="B9" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>45</v>
       </c>
       <c r="D9">
@@ -2381,7 +2380,7 @@
       <c r="E9">
         <v>255</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>1.14E-7</v>
       </c>
       <c r="G9">
@@ -2437,7 +2436,7 @@
       <c r="B10" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>48</v>
       </c>
       <c r="D10">
@@ -2482,8 +2481,8 @@
       <c r="Q10" t="s">
         <v>24</v>
       </c>
-      <c r="R10">
-        <v>8.82</v>
+      <c r="R10" t="s">
+        <v>24</v>
       </c>
       <c r="S10" t="s">
         <v>24</v>
@@ -2502,7 +2501,7 @@
       <c r="B11" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>51</v>
       </c>
       <c r="D11">
@@ -2511,7 +2510,7 @@
       <c r="E11">
         <v>343</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>1.6699999999999999E-10</v>
       </c>
       <c r="G11">
@@ -2523,7 +2522,7 @@
       <c r="I11">
         <v>205</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="1">
         <v>3.6900000000000002E-10</v>
       </c>
       <c r="K11">
@@ -2545,7 +2544,7 @@
         <v>6.25</v>
       </c>
       <c r="Q11">
-        <v>5.6300000000000003E-2</v>
+        <v>5.7200000000000001E-2</v>
       </c>
       <c r="R11">
         <v>3.5</v>
@@ -2567,7 +2566,7 @@
       <c r="B12" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>54</v>
       </c>
       <c r="D12">
@@ -2576,7 +2575,7 @@
       <c r="E12">
         <v>244</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>1.13E-9</v>
       </c>
       <c r="G12">
@@ -2588,7 +2587,7 @@
       <c r="I12">
         <v>137</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="1">
         <v>6.99E-7</v>
       </c>
       <c r="K12">
@@ -2610,7 +2609,7 @@
         <v>6.25</v>
       </c>
       <c r="Q12">
-        <v>0.32300000000000001</v>
+        <v>0.314</v>
       </c>
       <c r="R12">
         <v>12.2</v>
@@ -2632,7 +2631,7 @@
       <c r="B13" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>57</v>
       </c>
       <c r="D13">
@@ -2641,7 +2640,7 @@
       <c r="E13">
         <v>298</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>8.3400000000000006E-9</v>
       </c>
       <c r="G13">
@@ -2653,7 +2652,7 @@
       <c r="I13">
         <v>39.5</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="1">
         <v>1.38E-5</v>
       </c>
       <c r="K13">
@@ -2675,7 +2674,7 @@
         <v>21.7</v>
       </c>
       <c r="Q13">
-        <v>0.115</v>
+        <v>0.11</v>
       </c>
       <c r="R13">
         <v>18.5</v>
@@ -2697,7 +2696,7 @@
       <c r="B14" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>60</v>
       </c>
       <c r="D14">
@@ -2706,7 +2705,7 @@
       <c r="E14">
         <v>208</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>4.42E-9</v>
       </c>
       <c r="G14">
@@ -2762,7 +2761,7 @@
       <c r="B15" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>63</v>
       </c>
       <c r="D15">
@@ -2805,10 +2804,10 @@
         <v>21.7</v>
       </c>
       <c r="Q15">
-        <v>6.9699999999999998E-2</v>
-      </c>
-      <c r="R15">
-        <v>10.9</v>
+        <v>7.0800000000000002E-2</v>
+      </c>
+      <c r="R15" t="s">
+        <v>24</v>
       </c>
       <c r="S15" t="s">
         <v>24</v>
@@ -2827,7 +2826,7 @@
       <c r="B16" t="s">
         <v>65</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>66</v>
       </c>
       <c r="D16">
@@ -2836,7 +2835,7 @@
       <c r="E16">
         <v>419</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>2.2300000000000001E-8</v>
       </c>
       <c r="G16">
@@ -2848,10 +2847,10 @@
       <c r="I16">
         <v>97</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="1">
         <v>8.5799999999999997E-9</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="1">
         <v>4.8099999999999997E-6</v>
       </c>
       <c r="L16">
@@ -2870,7 +2869,7 @@
         <v>21.7</v>
       </c>
       <c r="Q16">
-        <v>4.8700000000000002E-3</v>
+        <v>4.7299999999999998E-3</v>
       </c>
       <c r="R16">
         <v>9.8800000000000008</v>
@@ -2892,7 +2891,7 @@
       <c r="B17" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>69</v>
       </c>
       <c r="D17">
@@ -2901,7 +2900,7 @@
       <c r="E17">
         <v>347</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>7.6599999999999995E-6</v>
       </c>
       <c r="G17">
@@ -2913,10 +2912,10 @@
       <c r="I17">
         <v>174</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="1">
         <v>1.9500000000000001E-7</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="1">
         <v>5.0099999999999998E-5</v>
       </c>
       <c r="L17">
@@ -2935,7 +2934,7 @@
         <v>21.7</v>
       </c>
       <c r="Q17">
-        <v>9.4399999999999998E-2</v>
+        <v>9.5799999999999996E-2</v>
       </c>
       <c r="R17">
         <v>2.77</v>
@@ -2957,7 +2956,7 @@
       <c r="B18" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>72</v>
       </c>
       <c r="D18">
@@ -2966,7 +2965,7 @@
       <c r="E18">
         <v>321</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>5.9399999999999997E-11</v>
       </c>
       <c r="G18">
@@ -2978,7 +2977,7 @@
       <c r="I18">
         <v>129</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="1">
         <v>8.2099999999999995E-7</v>
       </c>
       <c r="K18">
@@ -3022,7 +3021,7 @@
       <c r="B19" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>75</v>
       </c>
       <c r="D19">
@@ -3031,7 +3030,7 @@
       <c r="E19">
         <v>495</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <v>4.5900000000000002E-7</v>
       </c>
       <c r="G19">
@@ -3043,10 +3042,10 @@
       <c r="I19">
         <v>177</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="1">
         <v>5.5100000000000002E-9</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="1">
         <v>7.7599999999999997E-9</v>
       </c>
       <c r="L19">
@@ -3061,14 +3060,14 @@
       <c r="O19">
         <v>2.2800000000000001E-2</v>
       </c>
-      <c r="P19" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>24</v>
-      </c>
-      <c r="R19">
-        <v>10.8</v>
+      <c r="P19">
+        <v>21.7</v>
+      </c>
+      <c r="Q19">
+        <v>2.2599999999999999E-2</v>
+      </c>
+      <c r="R19" t="s">
+        <v>24</v>
       </c>
       <c r="S19" t="s">
         <v>24</v>
@@ -3087,7 +3086,7 @@
       <c r="B20" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>78</v>
       </c>
       <c r="D20">
@@ -3096,7 +3095,7 @@
       <c r="E20">
         <v>312</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>4.2199999999999999E-10</v>
       </c>
       <c r="G20">
@@ -3108,17 +3107,17 @@
       <c r="I20">
         <v>155</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="1">
         <v>4.3599999999999999E-7</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="1">
         <v>4.99E-5</v>
       </c>
       <c r="L20">
         <v>5.4</v>
       </c>
       <c r="M20">
-        <v>6.8000000000000005E-2</v>
+        <v>6.7599999999999993E-2</v>
       </c>
       <c r="N20">
         <v>16.3</v>
@@ -3130,10 +3129,10 @@
         <v>21.7</v>
       </c>
       <c r="Q20">
-        <v>6.9000000000000006E-2</v>
+        <v>5.5800000000000002E-2</v>
       </c>
       <c r="R20">
-        <v>5.97</v>
+        <v>5.96</v>
       </c>
       <c r="S20">
         <v>6.6600000000000006E-2</v>
@@ -3152,7 +3151,7 @@
       <c r="B21" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>81</v>
       </c>
       <c r="D21">
@@ -3161,7 +3160,7 @@
       <c r="E21">
         <v>194</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>8.3899999999999994E-9</v>
       </c>
       <c r="G21">
@@ -3217,7 +3216,7 @@
       <c r="B22" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>84</v>
       </c>
       <c r="D22">
@@ -3238,10 +3237,10 @@
       <c r="I22">
         <v>232</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="1">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="1">
         <v>2.11E-8</v>
       </c>
       <c r="L22" t="s">
@@ -3262,8 +3261,8 @@
       <c r="Q22" t="s">
         <v>24</v>
       </c>
-      <c r="R22">
-        <v>10.3</v>
+      <c r="R22" t="s">
+        <v>24</v>
       </c>
       <c r="S22" t="s">
         <v>24</v>
@@ -3282,7 +3281,7 @@
       <c r="B23" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>87</v>
       </c>
       <c r="D23">
@@ -3306,7 +3305,7 @@
       <c r="J23">
         <v>4.5199999999999997E-2</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="1">
         <v>1.5400000000000001E-6</v>
       </c>
       <c r="L23" t="s">
@@ -3327,8 +3326,8 @@
       <c r="Q23" t="s">
         <v>24</v>
       </c>
-      <c r="R23">
-        <v>9.26</v>
+      <c r="R23" t="s">
+        <v>24</v>
       </c>
       <c r="S23" t="s">
         <v>24</v>
@@ -3347,7 +3346,7 @@
       <c r="B24" t="s">
         <v>89</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>90</v>
       </c>
       <c r="D24">
@@ -3356,7 +3355,7 @@
       <c r="E24">
         <v>385</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>9.1200000000000008E-6</v>
       </c>
       <c r="G24">
@@ -3368,10 +3367,10 @@
       <c r="I24">
         <v>303</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J24" s="1">
         <v>1.5199999999999999E-9</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K24" s="1">
         <v>3.1200000000000001E-10</v>
       </c>
       <c r="L24" t="s">
@@ -3392,8 +3391,8 @@
       <c r="Q24" t="s">
         <v>24</v>
       </c>
-      <c r="R24">
-        <v>13.4</v>
+      <c r="R24" t="s">
+        <v>24</v>
       </c>
       <c r="S24" t="s">
         <v>24</v>
@@ -3412,7 +3411,7 @@
       <c r="B25" t="s">
         <v>92</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>93</v>
       </c>
       <c r="D25">
@@ -3457,8 +3456,8 @@
       <c r="Q25" t="s">
         <v>24</v>
       </c>
-      <c r="R25">
-        <v>8.82</v>
+      <c r="R25" t="s">
+        <v>24</v>
       </c>
       <c r="S25" t="s">
         <v>24</v>
@@ -3477,7 +3476,7 @@
       <c r="B26" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>96</v>
       </c>
       <c r="D26">
@@ -3486,7 +3485,7 @@
       <c r="E26">
         <v>64.7</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="1">
         <v>4.5600000000000004E-6</v>
       </c>
       <c r="G26">
@@ -3542,7 +3541,7 @@
       <c r="B27" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>99</v>
       </c>
       <c r="D27">
@@ -3551,7 +3550,7 @@
       <c r="E27">
         <v>340</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="1">
         <v>1.7999999999999999E-6</v>
       </c>
       <c r="G27">
@@ -3563,10 +3562,10 @@
       <c r="I27">
         <v>-34.4</v>
       </c>
-      <c r="J27" s="2">
+      <c r="J27" s="1">
         <v>2.02E-5</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K27" s="1">
         <v>4.0099999999999999E-5</v>
       </c>
       <c r="L27">
@@ -3585,10 +3584,10 @@
         <v>21.7</v>
       </c>
       <c r="Q27">
-        <v>2.1299999999999999E-2</v>
-      </c>
-      <c r="R27">
-        <v>10.4</v>
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="R27" t="s">
+        <v>24</v>
       </c>
       <c r="S27" t="s">
         <v>24</v>
@@ -3607,7 +3606,7 @@
       <c r="B28" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>102</v>
       </c>
       <c r="D28">
@@ -3616,7 +3615,7 @@
       <c r="E28">
         <v>353</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="1">
         <v>5.3400000000000002E-10</v>
       </c>
       <c r="G28">
@@ -3628,17 +3627,17 @@
       <c r="I28">
         <v>118</v>
       </c>
-      <c r="J28" s="2">
+      <c r="J28" s="1">
         <v>2.23E-7</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K28" s="1">
         <v>4.1999999999999998E-5</v>
       </c>
       <c r="L28">
         <v>3.79</v>
       </c>
       <c r="M28">
-        <v>3.6999999999999998E-2</v>
+        <v>3.6700000000000003E-2</v>
       </c>
       <c r="N28">
         <v>25.4</v>
@@ -3650,13 +3649,13 @@
         <v>21.7</v>
       </c>
       <c r="Q28">
-        <v>0.04</v>
+        <v>1.6899999999999998E-2</v>
       </c>
       <c r="R28">
         <v>4.46</v>
       </c>
       <c r="S28">
-        <v>3.73E-2</v>
+        <v>3.7199999999999997E-2</v>
       </c>
       <c r="T28">
         <v>3.8</v>
@@ -3672,7 +3671,7 @@
       <c r="B29" t="s">
         <v>104</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>105</v>
       </c>
       <c r="D29">
@@ -3681,7 +3680,7 @@
       <c r="E29">
         <v>350</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="1">
         <v>8.1300000000000007E-9</v>
       </c>
       <c r="G29">
@@ -3693,7 +3692,7 @@
       <c r="I29">
         <v>76</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J29" s="1">
         <v>6.7599999999999997E-7</v>
       </c>
       <c r="K29">
@@ -3703,7 +3702,7 @@
         <v>29</v>
       </c>
       <c r="M29">
-        <v>0.13700000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="N29">
         <v>19.399999999999999</v>
@@ -3715,7 +3714,7 @@
         <v>21.7</v>
       </c>
       <c r="Q29">
-        <v>9.98E-2</v>
+        <v>9.7900000000000001E-2</v>
       </c>
       <c r="R29">
         <v>16.7</v>
@@ -3737,7 +3736,7 @@
       <c r="B30" t="s">
         <v>107</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>108</v>
       </c>
       <c r="D30">
@@ -3746,7 +3745,7 @@
       <c r="E30">
         <v>332</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="1">
         <v>8.9900000000000003E-6</v>
       </c>
       <c r="G30">
@@ -3758,16 +3757,16 @@
       <c r="I30">
         <v>-39.799999999999997</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J30" s="1">
         <v>1.2100000000000001E-6</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K30" s="1">
         <v>1.04E-6</v>
       </c>
       <c r="L30">
         <v>45.9</v>
       </c>
-      <c r="M30" s="2">
+      <c r="M30" s="1">
         <v>2.3099999999999998E-8</v>
       </c>
       <c r="N30">
@@ -3780,10 +3779,10 @@
         <v>21.7</v>
       </c>
       <c r="Q30">
-        <v>5.6800000000000003E-2</v>
-      </c>
-      <c r="R30">
-        <v>10.6</v>
+        <v>5.57E-2</v>
+      </c>
+      <c r="R30" t="s">
+        <v>24</v>
       </c>
       <c r="S30" t="s">
         <v>24</v>
@@ -3802,7 +3801,7 @@
       <c r="B31" t="s">
         <v>110</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>111</v>
       </c>
       <c r="D31">
@@ -3811,7 +3810,7 @@
       <c r="E31">
         <v>335</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="1">
         <v>1.05E-8</v>
       </c>
       <c r="G31">
@@ -3823,7 +3822,7 @@
       <c r="I31">
         <v>119</v>
       </c>
-      <c r="J31" s="2">
+      <c r="J31" s="1">
         <v>2.7399999999999999E-7</v>
       </c>
       <c r="K31">
@@ -3845,13 +3844,13 @@
         <v>6.25</v>
       </c>
       <c r="Q31">
-        <v>0.122</v>
+        <v>9.9099999999999994E-2</v>
       </c>
       <c r="R31">
         <v>13.6</v>
       </c>
       <c r="S31">
-        <v>4.5100000000000001E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="T31">
         <v>30.1</v>
@@ -3867,7 +3866,7 @@
       <c r="B32" t="s">
         <v>113</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>114</v>
       </c>
       <c r="D32">
@@ -3876,7 +3875,7 @@
       <c r="E32">
         <v>377</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="1">
         <v>3.0499999999999999E-7</v>
       </c>
       <c r="G32">
@@ -3888,10 +3887,10 @@
       <c r="I32">
         <v>285</v>
       </c>
-      <c r="J32" s="2">
+      <c r="J32" s="1">
         <v>1.1600000000000001E-7</v>
       </c>
-      <c r="K32" s="2">
+      <c r="K32" s="1">
         <v>3.2899999999999998E-6</v>
       </c>
       <c r="L32" t="s">
@@ -3910,10 +3909,10 @@
         <v>21.7</v>
       </c>
       <c r="Q32">
-        <v>5.7799999999999997E-2</v>
-      </c>
-      <c r="R32">
-        <v>12.4</v>
+        <v>6.7900000000000002E-2</v>
+      </c>
+      <c r="R32" t="s">
+        <v>24</v>
       </c>
       <c r="S32" t="s">
         <v>24</v>
@@ -3932,7 +3931,7 @@
       <c r="B33" t="s">
         <v>116</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>117</v>
       </c>
       <c r="D33">
@@ -3977,8 +3976,8 @@
       <c r="Q33" t="s">
         <v>24</v>
       </c>
-      <c r="R33">
-        <v>10.4</v>
+      <c r="R33" t="s">
+        <v>24</v>
       </c>
       <c r="S33" t="s">
         <v>24</v>
@@ -3997,7 +3996,7 @@
       <c r="B34" t="s">
         <v>119</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>120</v>
       </c>
       <c r="D34">
@@ -4006,7 +4005,7 @@
       <c r="E34">
         <v>327</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="1">
         <v>2.4800000000000002E-10</v>
       </c>
       <c r="G34">
@@ -4018,7 +4017,7 @@
       <c r="I34">
         <v>65.5</v>
       </c>
-      <c r="J34" s="2">
+      <c r="J34" s="1">
         <v>2.3099999999999999E-7</v>
       </c>
       <c r="K34">
@@ -4040,7 +4039,7 @@
         <v>21.7</v>
       </c>
       <c r="Q34">
-        <v>2.86E-2</v>
+        <v>2.7099999999999999E-2</v>
       </c>
       <c r="R34">
         <v>16.100000000000001</v>
@@ -4062,7 +4061,7 @@
       <c r="B35" t="s">
         <v>122</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>123</v>
       </c>
       <c r="D35">
@@ -4071,7 +4070,7 @@
       <c r="E35">
         <v>207</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="1">
         <v>9.0799999999999998E-5</v>
       </c>
       <c r="G35">
@@ -4105,10 +4104,10 @@
         <v>21.7</v>
       </c>
       <c r="Q35">
-        <v>0.216</v>
-      </c>
-      <c r="R35">
-        <v>11.6</v>
+        <v>0.22</v>
+      </c>
+      <c r="R35" t="s">
+        <v>24</v>
       </c>
       <c r="S35" t="s">
         <v>24</v>
@@ -4127,7 +4126,7 @@
       <c r="B36" t="s">
         <v>125</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
         <v>126</v>
       </c>
       <c r="D36">
@@ -4136,7 +4135,7 @@
       <c r="E36">
         <v>205</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F36" s="1">
         <v>1.5E-10</v>
       </c>
       <c r="G36">
@@ -4192,7 +4191,7 @@
       <c r="B37" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" t="s">
         <v>129</v>
       </c>
       <c r="D37">
@@ -4201,7 +4200,7 @@
       <c r="E37">
         <v>168</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37" s="1">
         <v>2.3500000000000002E-10</v>
       </c>
       <c r="G37">
@@ -4216,7 +4215,7 @@
       <c r="J37">
         <v>0.90300000000000002</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K37" s="1">
         <v>9.1100000000000005E-5</v>
       </c>
       <c r="L37">
@@ -4257,7 +4256,7 @@
       <c r="B38" t="s">
         <v>131</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" t="s">
         <v>132</v>
       </c>
       <c r="D38">
@@ -4266,7 +4265,7 @@
       <c r="E38">
         <v>367</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F38" s="1">
         <v>5.9500000000000003E-5</v>
       </c>
       <c r="G38">
@@ -4278,10 +4277,10 @@
       <c r="I38">
         <v>98.9</v>
       </c>
-      <c r="J38" s="2">
+      <c r="J38" s="1">
         <v>8.0399999999999993E-6</v>
       </c>
-      <c r="K38" s="2">
+      <c r="K38" s="1">
         <v>2.77E-8</v>
       </c>
       <c r="L38" t="s">
@@ -4322,7 +4321,7 @@
       <c r="B39" t="s">
         <v>134</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" t="s">
         <v>135</v>
       </c>
       <c r="D39">
@@ -4331,7 +4330,7 @@
       <c r="E39">
         <v>332</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F39" s="1">
         <v>6.4299999999999995E-10</v>
       </c>
       <c r="G39">
@@ -4343,7 +4342,7 @@
       <c r="I39">
         <v>205</v>
       </c>
-      <c r="J39" s="2">
+      <c r="J39" s="1">
         <v>4.51E-7</v>
       </c>
       <c r="K39">
@@ -4365,7 +4364,7 @@
         <v>6.25</v>
       </c>
       <c r="Q39">
-        <v>0.20399999999999999</v>
+        <v>0.23699999999999999</v>
       </c>
       <c r="R39">
         <v>7.56</v>
@@ -4387,7 +4386,7 @@
       <c r="B40" t="s">
         <v>137</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>138</v>
       </c>
       <c r="D40">
@@ -4396,7 +4395,7 @@
       <c r="E40">
         <v>211</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40" s="1">
         <v>2.9500000000000002E-10</v>
       </c>
       <c r="G40">
@@ -4408,7 +4407,7 @@
       <c r="I40">
         <v>188</v>
       </c>
-      <c r="J40" s="2">
+      <c r="J40" s="1">
         <v>1.14E-8</v>
       </c>
       <c r="K40">
@@ -4452,7 +4451,7 @@
       <c r="B41" t="s">
         <v>140</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" t="s">
         <v>141</v>
       </c>
       <c r="D41">
@@ -4461,7 +4460,7 @@
       <c r="E41">
         <v>238</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="1">
         <v>1.94E-10</v>
       </c>
       <c r="G41">
@@ -4473,7 +4472,7 @@
       <c r="I41">
         <v>231</v>
       </c>
-      <c r="J41" s="2">
+      <c r="J41" s="1">
         <v>8.1899999999999992E-9</v>
       </c>
       <c r="K41">
@@ -4517,7 +4516,7 @@
       <c r="B42" t="s">
         <v>143</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" t="s">
         <v>144</v>
       </c>
       <c r="D42">
@@ -4526,7 +4525,7 @@
       <c r="E42">
         <v>180</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42" s="1">
         <v>3.1599999999999998E-8</v>
       </c>
       <c r="G42">
@@ -4582,7 +4581,7 @@
       <c r="B43" t="s">
         <v>146</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" t="s">
         <v>147</v>
       </c>
       <c r="D43">
@@ -4591,7 +4590,7 @@
       <c r="E43">
         <v>342</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F43" s="1">
         <v>1.27E-9</v>
       </c>
       <c r="G43">
@@ -4603,10 +4602,10 @@
       <c r="I43">
         <v>183</v>
       </c>
-      <c r="J43" s="2">
+      <c r="J43" s="1">
         <v>2.5799999999999999E-8</v>
       </c>
-      <c r="K43" s="2">
+      <c r="K43" s="1">
         <v>1.2E-9</v>
       </c>
       <c r="L43" t="s">
@@ -4647,7 +4646,7 @@
       <c r="B44" t="s">
         <v>149</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" t="s">
         <v>150</v>
       </c>
       <c r="D44">
@@ -4656,7 +4655,7 @@
       <c r="E44">
         <v>348</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F44" s="1">
         <v>1.42E-10</v>
       </c>
       <c r="G44">
@@ -4668,10 +4667,10 @@
       <c r="I44">
         <v>216</v>
       </c>
-      <c r="J44" s="2">
+      <c r="J44" s="1">
         <v>8.5800000000000004E-11</v>
       </c>
-      <c r="K44" s="2">
+      <c r="K44" s="1">
         <v>3.2400000000000001E-5</v>
       </c>
       <c r="L44">
@@ -4690,7 +4689,7 @@
         <v>6.25</v>
       </c>
       <c r="Q44">
-        <v>3.2199999999999999E-2</v>
+        <v>3.6200000000000003E-2</v>
       </c>
       <c r="R44">
         <v>8.94</v>
@@ -4712,7 +4711,7 @@
       <c r="B45" t="s">
         <v>152</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" t="s">
         <v>153</v>
       </c>
       <c r="D45">
@@ -4721,7 +4720,7 @@
       <c r="E45">
         <v>364</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F45" s="1">
         <v>2.92E-6</v>
       </c>
       <c r="G45">
@@ -4733,10 +4732,10 @@
       <c r="I45">
         <v>42</v>
       </c>
-      <c r="J45" s="2">
+      <c r="J45" s="1">
         <v>2.0299999999999999E-5</v>
       </c>
-      <c r="K45" s="2">
+      <c r="K45" s="1">
         <v>3.2899999999999998E-6</v>
       </c>
       <c r="L45">
@@ -4755,7 +4754,7 @@
         <v>21.7</v>
       </c>
       <c r="Q45">
-        <v>9.58E-3</v>
+        <v>9.5899999999999996E-3</v>
       </c>
       <c r="R45">
         <v>12.4</v>
@@ -4777,7 +4776,7 @@
       <c r="B46" t="s">
         <v>155</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" t="s">
         <v>156</v>
       </c>
       <c r="D46">
@@ -4786,7 +4785,7 @@
       <c r="E46">
         <v>102</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F46" s="1">
         <v>4.8999999999999997E-6</v>
       </c>
       <c r="G46">
@@ -4822,8 +4821,8 @@
       <c r="Q46" t="s">
         <v>24</v>
       </c>
-      <c r="R46">
-        <v>7.83</v>
+      <c r="R46" t="s">
+        <v>24</v>
       </c>
       <c r="S46" t="s">
         <v>24</v>
@@ -4842,7 +4841,7 @@
       <c r="B47" t="s">
         <v>158</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" t="s">
         <v>159</v>
       </c>
       <c r="D47">
@@ -4851,7 +4850,7 @@
       <c r="E47">
         <v>334</v>
       </c>
-      <c r="F47" s="2">
+      <c r="F47" s="1">
         <v>1.8600000000000001E-8</v>
       </c>
       <c r="G47">
@@ -4863,10 +4862,10 @@
       <c r="I47">
         <v>226</v>
       </c>
-      <c r="J47" s="2">
+      <c r="J47" s="1">
         <v>2.2399999999999999E-8</v>
       </c>
-      <c r="K47" s="2">
+      <c r="K47" s="1">
         <v>4.3000000000000002E-5</v>
       </c>
       <c r="L47">
@@ -4885,7 +4884,7 @@
         <v>6.25</v>
       </c>
       <c r="Q47">
-        <v>0.26400000000000001</v>
+        <v>0.26</v>
       </c>
       <c r="R47">
         <v>6.42</v>
@@ -4907,7 +4906,7 @@
       <c r="B48" t="s">
         <v>161</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" t="s">
         <v>162</v>
       </c>
       <c r="D48">
@@ -4916,7 +4915,7 @@
       <c r="E48">
         <v>267</v>
       </c>
-      <c r="F48" s="2">
+      <c r="F48" s="1">
         <v>6.4000000000000001E-7</v>
       </c>
       <c r="G48">
@@ -4972,7 +4971,7 @@
       <c r="B49" t="s">
         <v>164</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" t="s">
         <v>165</v>
       </c>
       <c r="D49">
@@ -4981,7 +4980,7 @@
       <c r="E49">
         <v>270</v>
       </c>
-      <c r="F49" s="2">
+      <c r="F49" s="1">
         <v>2.98E-9</v>
       </c>
       <c r="G49">
@@ -4993,7 +4992,7 @@
       <c r="I49">
         <v>96.8</v>
       </c>
-      <c r="J49" s="2">
+      <c r="J49" s="1">
         <v>6.0000000000000002E-6</v>
       </c>
       <c r="K49">
@@ -5015,7 +5014,7 @@
         <v>21.7</v>
       </c>
       <c r="Q49">
-        <v>9.3899999999999997E-2</v>
+        <v>9.6299999999999997E-2</v>
       </c>
       <c r="R49">
         <v>33.1</v>
@@ -5037,7 +5036,7 @@
       <c r="B50" t="s">
         <v>167</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" t="s">
         <v>168</v>
       </c>
       <c r="D50">
@@ -5046,7 +5045,7 @@
       <c r="E50">
         <v>337</v>
       </c>
-      <c r="F50" s="2">
+      <c r="F50" s="1">
         <v>5.9799999999999996E-9</v>
       </c>
       <c r="G50">
@@ -5058,7 +5057,7 @@
       <c r="I50">
         <v>213</v>
       </c>
-      <c r="J50" s="2">
+      <c r="J50" s="1">
         <v>6.9900000000000001E-9</v>
       </c>
       <c r="K50">
@@ -5080,7 +5079,7 @@
         <v>6.25</v>
       </c>
       <c r="Q50">
-        <v>0.20799999999999999</v>
+        <v>0.19</v>
       </c>
       <c r="R50">
         <v>6.42</v>
@@ -5102,7 +5101,7 @@
       <c r="B51" t="s">
         <v>170</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" t="s">
         <v>171</v>
       </c>
       <c r="D51">
@@ -5111,7 +5110,7 @@
       <c r="E51">
         <v>218</v>
       </c>
-      <c r="F51" s="2">
+      <c r="F51" s="1">
         <v>3.9100000000000002E-5</v>
       </c>
       <c r="G51">
@@ -5141,14 +5140,14 @@
       <c r="O51">
         <v>0.54400000000000004</v>
       </c>
-      <c r="P51" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q51" t="s">
-        <v>24</v>
-      </c>
-      <c r="R51">
-        <v>10.6</v>
+      <c r="P51">
+        <v>21.7</v>
+      </c>
+      <c r="Q51">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="R51" t="s">
+        <v>24</v>
       </c>
       <c r="S51" t="s">
         <v>24</v>
@@ -5167,7 +5166,7 @@
       <c r="B52" t="s">
         <v>173</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" t="s">
         <v>174</v>
       </c>
       <c r="D52">
@@ -5176,7 +5175,7 @@
       <c r="E52">
         <v>215</v>
       </c>
-      <c r="F52" s="2">
+      <c r="F52" s="1">
         <v>7.0100000000000004E-9</v>
       </c>
       <c r="G52">
@@ -5232,7 +5231,7 @@
       <c r="B53" t="s">
         <v>176</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" t="s">
         <v>177</v>
       </c>
       <c r="D53">
@@ -5241,7 +5240,7 @@
       <c r="E53">
         <v>275</v>
       </c>
-      <c r="F53" s="2">
+      <c r="F53" s="1">
         <v>1.3999999999999999E-9</v>
       </c>
       <c r="G53">
@@ -5253,10 +5252,10 @@
       <c r="I53">
         <v>211</v>
       </c>
-      <c r="J53" s="2">
+      <c r="J53" s="1">
         <v>7.5899999999999996E-10</v>
       </c>
-      <c r="K53" s="2">
+      <c r="K53" s="1">
         <v>7.9900000000000004E-5</v>
       </c>
       <c r="L53">
@@ -5275,7 +5274,7 @@
         <v>21.7</v>
       </c>
       <c r="Q53">
-        <v>0.38100000000000001</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="R53">
         <v>15</v>
@@ -5297,7 +5296,7 @@
       <c r="B54" t="s">
         <v>179</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" t="s">
         <v>180</v>
       </c>
       <c r="D54">
@@ -5306,7 +5305,7 @@
       <c r="E54">
         <v>294</v>
       </c>
-      <c r="F54" s="2">
+      <c r="F54" s="1">
         <v>8.1100000000000005E-8</v>
       </c>
       <c r="G54">
@@ -5340,7 +5339,7 @@
         <v>21.7</v>
       </c>
       <c r="Q54">
-        <v>0.23400000000000001</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="R54">
         <v>13.1</v>
@@ -5362,7 +5361,7 @@
       <c r="B55" t="s">
         <v>182</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" t="s">
         <v>183</v>
       </c>
       <c r="D55">
@@ -5371,7 +5370,7 @@
       <c r="E55">
         <v>314</v>
       </c>
-      <c r="F55" s="2">
+      <c r="F55" s="1">
         <v>3.0399999999999998E-9</v>
       </c>
       <c r="G55">
@@ -5383,7 +5382,7 @@
       <c r="I55">
         <v>121</v>
       </c>
-      <c r="J55" s="2">
+      <c r="J55" s="1">
         <v>1.22E-8</v>
       </c>
       <c r="K55">
@@ -5405,7 +5404,7 @@
         <v>6.25</v>
       </c>
       <c r="Q55">
-        <v>0.749</v>
+        <v>0.748</v>
       </c>
       <c r="R55">
         <v>9.25</v>
@@ -5427,7 +5426,7 @@
       <c r="B56" t="s">
         <v>185</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" t="s">
         <v>186</v>
       </c>
       <c r="D56">
@@ -5472,8 +5471,8 @@
       <c r="Q56" t="s">
         <v>24</v>
       </c>
-      <c r="R56">
-        <v>8.5</v>
+      <c r="R56" t="s">
+        <v>24</v>
       </c>
       <c r="S56" t="s">
         <v>24</v>
@@ -5492,7 +5491,7 @@
       <c r="B57" t="s">
         <v>188</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" t="s">
         <v>189</v>
       </c>
       <c r="D57">
@@ -5501,7 +5500,7 @@
       <c r="E57">
         <v>127</v>
       </c>
-      <c r="F57" s="2">
+      <c r="F57" s="1">
         <v>6.2700000000000001E-6</v>
       </c>
       <c r="G57">
@@ -5557,7 +5556,7 @@
       <c r="B58" t="s">
         <v>191</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" t="s">
         <v>192</v>
       </c>
       <c r="D58">
@@ -5566,7 +5565,7 @@
       <c r="E58">
         <v>281</v>
       </c>
-      <c r="F58" s="2">
+      <c r="F58" s="1">
         <v>8.1899999999999999E-8</v>
       </c>
       <c r="G58">
@@ -5600,7 +5599,7 @@
         <v>21.7</v>
       </c>
       <c r="Q58">
-        <v>1.5100000000000001E-2</v>
+        <v>1.8499999999999999E-2</v>
       </c>
       <c r="R58">
         <v>7.05</v>
@@ -5622,7 +5621,7 @@
       <c r="B59" t="s">
         <v>194</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" t="s">
         <v>195</v>
       </c>
       <c r="D59">
@@ -5631,7 +5630,7 @@
       <c r="E59">
         <v>350</v>
       </c>
-      <c r="F59" s="2">
+      <c r="F59" s="1">
         <v>6.1300000000000001E-9</v>
       </c>
       <c r="G59">
@@ -5643,10 +5642,10 @@
       <c r="I59">
         <v>159</v>
       </c>
-      <c r="J59" s="2">
+      <c r="J59" s="1">
         <v>1.33E-9</v>
       </c>
-      <c r="K59" s="2">
+      <c r="K59" s="1">
         <v>5.0899999999999997E-5</v>
       </c>
       <c r="L59">
@@ -5687,7 +5686,7 @@
       <c r="B60" t="s">
         <v>197</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" t="s">
         <v>198</v>
       </c>
       <c r="D60">
@@ -5696,7 +5695,7 @@
       <c r="E60">
         <v>324</v>
       </c>
-      <c r="F60" s="2">
+      <c r="F60" s="1">
         <v>2.0799999999999998E-9</v>
       </c>
       <c r="G60">
@@ -5708,10 +5707,10 @@
       <c r="I60">
         <v>179</v>
       </c>
-      <c r="J60" s="2">
+      <c r="J60" s="1">
         <v>4.0399999999999998E-8</v>
       </c>
-      <c r="K60" s="2">
+      <c r="K60" s="1">
         <v>9.0099999999999995E-5</v>
       </c>
       <c r="L60" t="s">
@@ -5730,7 +5729,7 @@
         <v>21.7</v>
       </c>
       <c r="Q60">
-        <v>7.8100000000000003E-2</v>
+        <v>6.93E-2</v>
       </c>
       <c r="R60">
         <v>15.7</v>
@@ -5752,7 +5751,7 @@
       <c r="B61" t="s">
         <v>200</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" t="s">
         <v>201</v>
       </c>
       <c r="D61">
@@ -5817,7 +5816,7 @@
       <c r="B62" t="s">
         <v>203</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" t="s">
         <v>204</v>
       </c>
       <c r="D62">
@@ -5826,7 +5825,7 @@
       <c r="E62">
         <v>389</v>
       </c>
-      <c r="F62" s="2">
+      <c r="F62" s="1">
         <v>1.7700000000000001E-10</v>
       </c>
       <c r="G62">
@@ -5838,10 +5837,10 @@
       <c r="I62">
         <v>257</v>
       </c>
-      <c r="J62" s="2">
+      <c r="J62" s="1">
         <v>8.3400000000000002E-10</v>
       </c>
-      <c r="K62" s="2">
+      <c r="K62" s="1">
         <v>2.0100000000000001E-5</v>
       </c>
       <c r="L62" t="s">
@@ -5860,7 +5859,7 @@
         <v>21.7</v>
       </c>
       <c r="Q62">
-        <v>4.87E-2</v>
+        <v>5.0599999999999999E-2</v>
       </c>
       <c r="R62">
         <v>13.9</v>
@@ -5882,7 +5881,7 @@
       <c r="B63" t="s">
         <v>206</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" t="s">
         <v>207</v>
       </c>
       <c r="D63">
@@ -5891,7 +5890,7 @@
       <c r="E63">
         <v>262</v>
       </c>
-      <c r="F63" s="2">
+      <c r="F63" s="1">
         <v>9.9300000000000001E-5</v>
       </c>
       <c r="G63">
@@ -5925,10 +5924,10 @@
         <v>21.7</v>
       </c>
       <c r="Q63">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="R63">
-        <v>20.9</v>
+        <v>0.157</v>
+      </c>
+      <c r="R63" t="s">
+        <v>24</v>
       </c>
       <c r="S63" t="s">
         <v>24</v>
@@ -5947,7 +5946,7 @@
       <c r="B64" t="s">
         <v>209</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" t="s">
         <v>210</v>
       </c>
       <c r="D64">
@@ -5956,7 +5955,7 @@
       <c r="E64">
         <v>200</v>
       </c>
-      <c r="F64" s="2">
+      <c r="F64" s="1">
         <v>7.9099999999999998E-5</v>
       </c>
       <c r="G64">
@@ -5990,10 +5989,10 @@
         <v>21.7</v>
       </c>
       <c r="Q64">
-        <v>0.189</v>
-      </c>
-      <c r="R64">
-        <v>11.3</v>
+        <v>0.246</v>
+      </c>
+      <c r="R64" t="s">
+        <v>24</v>
       </c>
       <c r="S64" t="s">
         <v>24</v>
@@ -6012,7 +6011,7 @@
       <c r="B65" t="s">
         <v>212</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" t="s">
         <v>213</v>
       </c>
       <c r="D65">
@@ -6021,7 +6020,7 @@
       <c r="E65">
         <v>323</v>
       </c>
-      <c r="F65" s="2">
+      <c r="F65" s="1">
         <v>1.9300000000000001E-10</v>
       </c>
       <c r="G65">
@@ -6033,7 +6032,7 @@
       <c r="I65">
         <v>144</v>
       </c>
-      <c r="J65" s="2">
+      <c r="J65" s="1">
         <v>4.3599999999999998E-9</v>
       </c>
       <c r="K65">
@@ -6055,13 +6054,13 @@
         <v>6.25</v>
       </c>
       <c r="Q65">
-        <v>0.58399999999999996</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="R65">
         <v>4.3</v>
       </c>
       <c r="S65">
-        <v>0.71299999999999997</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="T65">
         <v>2.81</v>
@@ -6077,7 +6076,7 @@
       <c r="B66" t="s">
         <v>215</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" t="s">
         <v>216</v>
       </c>
       <c r="D66">
@@ -6086,7 +6085,7 @@
       <c r="E66">
         <v>342</v>
       </c>
-      <c r="F66" s="2">
+      <c r="F66" s="1">
         <v>6.5200000000000002E-10</v>
       </c>
       <c r="G66">
@@ -6098,10 +6097,10 @@
       <c r="I66">
         <v>55.8</v>
       </c>
-      <c r="J66" s="2">
+      <c r="J66" s="1">
         <v>2.4600000000000001E-7</v>
       </c>
-      <c r="K66" s="2">
+      <c r="K66" s="1">
         <v>3.4499999999999998E-5</v>
       </c>
       <c r="L66">
@@ -6120,7 +6119,7 @@
         <v>21.7</v>
       </c>
       <c r="Q66">
-        <v>4.7099999999999998E-3</v>
+        <v>6.1999999999999998E-3</v>
       </c>
       <c r="R66">
         <v>16.3</v>
@@ -6142,7 +6141,7 @@
       <c r="B67" t="s">
         <v>218</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" t="s">
         <v>219</v>
       </c>
       <c r="D67">
@@ -6151,7 +6150,7 @@
       <c r="E67">
         <v>294</v>
       </c>
-      <c r="F67" s="2">
+      <c r="F67" s="1">
         <v>2.01E-10</v>
       </c>
       <c r="G67">
@@ -6163,14 +6162,14 @@
       <c r="I67">
         <v>119</v>
       </c>
-      <c r="J67" s="2">
+      <c r="J67" s="1">
         <v>5.1499999999999998E-9</v>
       </c>
       <c r="K67">
         <v>1.75E-4</v>
       </c>
       <c r="L67">
-        <v>0.34</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="M67">
         <v>0.98399999999999999</v>
@@ -6185,7 +6184,7 @@
         <v>6.25</v>
       </c>
       <c r="Q67">
-        <v>0.46400000000000002</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="R67">
         <v>10.6</v>
@@ -6207,7 +6206,7 @@
       <c r="B68" t="s">
         <v>221</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" t="s">
         <v>222</v>
       </c>
       <c r="D68">
@@ -6216,7 +6215,7 @@
       <c r="E68">
         <v>241</v>
       </c>
-      <c r="F68" s="2">
+      <c r="F68" s="1">
         <v>1.1200000000000001E-11</v>
       </c>
       <c r="G68">
@@ -6228,17 +6227,17 @@
       <c r="I68">
         <v>178</v>
       </c>
-      <c r="J68" s="2">
+      <c r="J68" s="1">
         <v>7.0600000000000004E-10</v>
       </c>
-      <c r="K68" s="2">
+      <c r="K68" s="1">
         <v>4.1199999999999998E-8</v>
       </c>
       <c r="L68">
         <v>2.87</v>
       </c>
-      <c r="M68">
-        <v>0</v>
+      <c r="M68" t="s">
+        <v>24</v>
       </c>
       <c r="N68">
         <v>24</v>
@@ -6250,7 +6249,7 @@
         <v>21.7</v>
       </c>
       <c r="Q68">
-        <v>7.7499999999999999E-3</v>
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="R68">
         <v>4.28</v>
@@ -6272,7 +6271,7 @@
       <c r="B69" t="s">
         <v>224</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" t="s">
         <v>225</v>
       </c>
       <c r="D69">
@@ -6281,7 +6280,7 @@
       <c r="E69">
         <v>331</v>
       </c>
-      <c r="F69" s="2">
+      <c r="F69" s="1">
         <v>2.7099999999999998E-7</v>
       </c>
       <c r="G69">
@@ -6293,7 +6292,7 @@
       <c r="I69">
         <v>63.6</v>
       </c>
-      <c r="J69" s="2">
+      <c r="J69" s="1">
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="K69">
@@ -6315,13 +6314,13 @@
         <v>21.7</v>
       </c>
       <c r="Q69">
-        <v>0.27600000000000002</v>
+        <v>0.29699999999999999</v>
       </c>
       <c r="R69">
         <v>18.5</v>
       </c>
       <c r="S69">
-        <v>0.28100000000000003</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="T69">
         <v>34.6</v>
@@ -6337,7 +6336,7 @@
       <c r="B70" t="s">
         <v>227</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" t="s">
         <v>228</v>
       </c>
       <c r="D70">
@@ -6346,7 +6345,7 @@
       <c r="E70">
         <v>394</v>
       </c>
-      <c r="F70" s="2">
+      <c r="F70" s="1">
         <v>1.7599999999999999E-9</v>
       </c>
       <c r="G70">
@@ -6358,7 +6357,7 @@
       <c r="I70">
         <v>210</v>
       </c>
-      <c r="J70" s="2">
+      <c r="J70" s="1">
         <v>1.89E-8</v>
       </c>
       <c r="K70">
@@ -6402,7 +6401,7 @@
       <c r="B71" t="s">
         <v>230</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" t="s">
         <v>231</v>
       </c>
       <c r="D71">
@@ -6447,8 +6446,8 @@
       <c r="Q71" t="s">
         <v>24</v>
       </c>
-      <c r="R71">
-        <v>9.68</v>
+      <c r="R71" t="s">
+        <v>24</v>
       </c>
       <c r="S71" t="s">
         <v>24</v>
@@ -6467,7 +6466,7 @@
       <c r="B72" t="s">
         <v>233</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" t="s">
         <v>234</v>
       </c>
       <c r="D72">
@@ -6476,7 +6475,7 @@
       <c r="E72">
         <v>319</v>
       </c>
-      <c r="F72" s="2">
+      <c r="F72" s="1">
         <v>2.65E-6</v>
       </c>
       <c r="G72">
@@ -6510,13 +6509,13 @@
         <v>6.25</v>
       </c>
       <c r="Q72">
-        <v>0.505</v>
+        <v>0.48899999999999999</v>
       </c>
       <c r="R72">
         <v>10</v>
       </c>
       <c r="S72">
-        <v>0.81299999999999994</v>
+        <v>0.81200000000000006</v>
       </c>
       <c r="T72">
         <v>0.51</v>
@@ -6532,7 +6531,7 @@
       <c r="B73" t="s">
         <v>236</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" t="s">
         <v>237</v>
       </c>
       <c r="D73">
@@ -6541,7 +6540,7 @@
       <c r="E73">
         <v>317</v>
       </c>
-      <c r="F73" s="2">
+      <c r="F73" s="1">
         <v>1.57E-10</v>
       </c>
       <c r="G73">
@@ -6553,17 +6552,17 @@
       <c r="I73">
         <v>234</v>
       </c>
-      <c r="J73" s="2">
+      <c r="J73" s="1">
         <v>2.6299999999999998E-9</v>
       </c>
-      <c r="K73" s="2">
+      <c r="K73" s="1">
         <v>6.1600000000000003E-6</v>
       </c>
       <c r="L73">
         <v>65.400000000000006</v>
       </c>
-      <c r="M73">
-        <v>5.0000000000000001E-3</v>
+      <c r="M73" t="s">
+        <v>24</v>
       </c>
       <c r="N73" t="s">
         <v>24</v>
@@ -6597,7 +6596,7 @@
       <c r="B74" t="s">
         <v>239</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" t="s">
         <v>240</v>
       </c>
       <c r="D74">
@@ -6606,7 +6605,7 @@
       <c r="E74">
         <v>222</v>
       </c>
-      <c r="F74" s="2">
+      <c r="F74" s="1">
         <v>8.3200000000000004E-7</v>
       </c>
       <c r="G74">
@@ -6625,7 +6624,7 @@
         <v>1.38E-2</v>
       </c>
       <c r="L74">
-        <v>0.44</v>
+        <v>0.437</v>
       </c>
       <c r="M74">
         <v>0.214</v>
@@ -6640,7 +6639,7 @@
         <v>0</v>
       </c>
       <c r="Q74">
-        <v>0.33400000000000002</v>
+        <v>0.30199999999999999</v>
       </c>
       <c r="R74">
         <v>13.8</v>
@@ -6662,7 +6661,7 @@
       <c r="B75" t="s">
         <v>242</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" t="s">
         <v>243</v>
       </c>
       <c r="D75">
@@ -6707,8 +6706,8 @@
       <c r="Q75" t="s">
         <v>24</v>
       </c>
-      <c r="R75">
-        <v>7.59</v>
+      <c r="R75" t="s">
+        <v>24</v>
       </c>
       <c r="S75" t="s">
         <v>24</v>
@@ -6727,7 +6726,7 @@
       <c r="B76" t="s">
         <v>245</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" t="s">
         <v>246</v>
       </c>
       <c r="D76">
@@ -6736,7 +6735,7 @@
       <c r="E76">
         <v>397</v>
       </c>
-      <c r="F76" s="2">
+      <c r="F76" s="1">
         <v>2.6700000000000001E-9</v>
       </c>
       <c r="G76">
@@ -6748,10 +6747,10 @@
       <c r="I76">
         <v>178</v>
       </c>
-      <c r="J76" s="2">
+      <c r="J76" s="1">
         <v>1.1700000000000001E-9</v>
       </c>
-      <c r="K76" s="2">
+      <c r="K76" s="1">
         <v>1.06E-5</v>
       </c>
       <c r="L76">
@@ -6770,7 +6769,7 @@
         <v>21.7</v>
       </c>
       <c r="Q76">
-        <v>3.4200000000000001E-2</v>
+        <v>3.7100000000000001E-2</v>
       </c>
       <c r="R76">
         <v>13.6</v>
@@ -6792,7 +6791,7 @@
       <c r="B77" t="s">
         <v>248</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" t="s">
         <v>249</v>
       </c>
       <c r="D77">
@@ -6801,7 +6800,7 @@
       <c r="E77">
         <v>227</v>
       </c>
-      <c r="F77" s="2">
+      <c r="F77" s="1">
         <v>1.4800000000000001E-9</v>
       </c>
       <c r="G77">
@@ -6820,10 +6819,10 @@
         <v>4.6100000000000003</v>
       </c>
       <c r="L77">
-        <v>5.81</v>
+        <v>5.82</v>
       </c>
       <c r="M77">
-        <v>0.84299999999999997</v>
+        <v>0.84399999999999997</v>
       </c>
       <c r="N77">
         <v>20.399999999999999</v>
@@ -6835,13 +6834,13 @@
         <v>0</v>
       </c>
       <c r="Q77">
-        <v>0.61599999999999999</v>
+        <v>0.627</v>
       </c>
       <c r="R77">
         <v>6.36</v>
       </c>
       <c r="S77">
-        <v>0.85699999999999998</v>
+        <v>0.85599999999999998</v>
       </c>
       <c r="T77">
         <v>5.81</v>
@@ -6857,7 +6856,7 @@
       <c r="B78" t="s">
         <v>251</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" t="s">
         <v>252</v>
       </c>
       <c r="D78">
@@ -6866,7 +6865,7 @@
       <c r="E78">
         <v>343</v>
       </c>
-      <c r="F78" s="2">
+      <c r="F78" s="1">
         <v>1.2499999999999999E-7</v>
       </c>
       <c r="G78">
@@ -6878,7 +6877,7 @@
       <c r="I78">
         <v>153</v>
       </c>
-      <c r="J78" s="2">
+      <c r="J78" s="1">
         <v>6.7799999999999998E-8</v>
       </c>
       <c r="K78">
@@ -6900,7 +6899,7 @@
         <v>21.7</v>
       </c>
       <c r="Q78">
-        <v>3.7600000000000001E-2</v>
+        <v>4.4499999999999998E-2</v>
       </c>
       <c r="R78">
         <v>17.8</v>
@@ -6922,7 +6921,7 @@
       <c r="B79" t="s">
         <v>254</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" t="s">
         <v>255</v>
       </c>
       <c r="D79">
@@ -6931,7 +6930,7 @@
       <c r="E79">
         <v>309</v>
       </c>
-      <c r="F79" s="2">
+      <c r="F79" s="1">
         <v>2.4599999999999999E-8</v>
       </c>
       <c r="G79">
@@ -6987,7 +6986,7 @@
       <c r="B80" t="s">
         <v>257</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" t="s">
         <v>258</v>
       </c>
       <c r="D80">
@@ -6996,7 +6995,7 @@
       <c r="E80">
         <v>362</v>
       </c>
-      <c r="F80" s="2">
+      <c r="F80" s="1">
         <v>3.25E-8</v>
       </c>
       <c r="G80">
@@ -7008,17 +7007,17 @@
       <c r="I80">
         <v>44.4</v>
       </c>
-      <c r="J80" s="2">
+      <c r="J80" s="1">
         <v>1.14E-8</v>
       </c>
-      <c r="K80" s="2">
+      <c r="K80" s="1">
         <v>2.2600000000000001E-7</v>
       </c>
       <c r="L80">
         <v>99</v>
       </c>
-      <c r="M80">
-        <v>0</v>
+      <c r="M80" t="s">
+        <v>24</v>
       </c>
       <c r="N80">
         <v>60.6</v>
@@ -7030,7 +7029,7 @@
         <v>21.7</v>
       </c>
       <c r="Q80">
-        <v>8.2299999999999995E-3</v>
+        <v>8.2799999999999992E-3</v>
       </c>
       <c r="R80">
         <v>14.1</v>
@@ -7052,7 +7051,7 @@
       <c r="B81" t="s">
         <v>260</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" t="s">
         <v>261</v>
       </c>
       <c r="D81">
@@ -7061,7 +7060,7 @@
       <c r="E81">
         <v>266</v>
       </c>
-      <c r="F81" s="2">
+      <c r="F81" s="1">
         <v>2.2100000000000001E-7</v>
       </c>
       <c r="G81">
@@ -7082,8 +7081,8 @@
       <c r="L81">
         <v>71.8</v>
       </c>
-      <c r="M81">
-        <v>0</v>
+      <c r="M81" t="s">
+        <v>24</v>
       </c>
       <c r="N81">
         <v>27.8</v>
@@ -7095,7 +7094,7 @@
         <v>21.7</v>
       </c>
       <c r="Q81">
-        <v>3.7699999999999997E-2</v>
+        <v>4.0599999999999997E-2</v>
       </c>
       <c r="R81">
         <v>16.5</v>
@@ -7117,7 +7116,7 @@
       <c r="B82" t="s">
         <v>263</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" t="s">
         <v>264</v>
       </c>
       <c r="D82">
@@ -7126,7 +7125,7 @@
       <c r="E82">
         <v>272</v>
       </c>
-      <c r="F82" s="2">
+      <c r="F82" s="1">
         <v>4.2599999999999998E-10</v>
       </c>
       <c r="G82">
@@ -7138,7 +7137,7 @@
       <c r="I82">
         <v>281</v>
       </c>
-      <c r="J82" s="2">
+      <c r="J82" s="1">
         <v>4.9299999999999998E-8</v>
       </c>
       <c r="K82">
@@ -7160,7 +7159,7 @@
         <v>6.25</v>
       </c>
       <c r="Q82">
-        <v>0.33800000000000002</v>
+        <v>0.33200000000000002</v>
       </c>
       <c r="R82">
         <v>4.93</v>
@@ -7182,7 +7181,7 @@
       <c r="B83" t="s">
         <v>266</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" t="s">
         <v>267</v>
       </c>
       <c r="D83">
@@ -7191,7 +7190,7 @@
       <c r="E83">
         <v>154</v>
       </c>
-      <c r="F83" s="2">
+      <c r="F83" s="1">
         <v>2.0700000000000001E-10</v>
       </c>
       <c r="G83">
@@ -7206,7 +7205,7 @@
       <c r="J83">
         <v>0.20699999999999999</v>
       </c>
-      <c r="K83" s="2">
+      <c r="K83" s="1">
         <v>4.1199999999999998E-7</v>
       </c>
       <c r="L83" t="s">
@@ -7247,7 +7246,7 @@
       <c r="B84" t="s">
         <v>269</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" t="s">
         <v>270</v>
       </c>
       <c r="D84">
@@ -7268,10 +7267,10 @@
       <c r="I84">
         <v>204</v>
       </c>
-      <c r="J84" s="2">
+      <c r="J84" s="1">
         <v>2.6000000000000001E-9</v>
       </c>
-      <c r="K84" s="2">
+      <c r="K84" s="1">
         <v>6.8700000000000001E-10</v>
       </c>
       <c r="L84" t="s">
@@ -7312,7 +7311,7 @@
       <c r="B85" t="s">
         <v>272</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" t="s">
         <v>273</v>
       </c>
       <c r="D85">
@@ -7321,7 +7320,7 @@
       <c r="E85">
         <v>327</v>
       </c>
-      <c r="F85" s="2">
+      <c r="F85" s="1">
         <v>1.27E-11</v>
       </c>
       <c r="G85">
@@ -7333,10 +7332,10 @@
       <c r="I85">
         <v>218</v>
       </c>
-      <c r="J85" s="2">
+      <c r="J85" s="1">
         <v>3.5200000000000003E-10</v>
       </c>
-      <c r="K85" s="2">
+      <c r="K85" s="1">
         <v>4.3900000000000003E-6</v>
       </c>
       <c r="L85">
@@ -7355,7 +7354,7 @@
         <v>21.7</v>
       </c>
       <c r="Q85">
-        <v>1.9199999999999998E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="R85">
         <v>3.83</v>
@@ -7377,7 +7376,7 @@
       <c r="B86" t="s">
         <v>275</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" t="s">
         <v>276</v>
       </c>
       <c r="D86">
@@ -7386,7 +7385,7 @@
       <c r="E86">
         <v>219</v>
       </c>
-      <c r="F86" s="2">
+      <c r="F86" s="1">
         <v>1.7999999999999999E-11</v>
       </c>
       <c r="G86">
@@ -7398,7 +7397,7 @@
       <c r="I86">
         <v>185</v>
       </c>
-      <c r="J86" s="2">
+      <c r="J86" s="1">
         <v>2.48E-6</v>
       </c>
       <c r="K86">
@@ -7442,7 +7441,7 @@
       <c r="B87" t="s">
         <v>278</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" t="s">
         <v>279</v>
       </c>
       <c r="D87">
@@ -7451,7 +7450,7 @@
       <c r="E87">
         <v>263</v>
       </c>
-      <c r="F87" s="2">
+      <c r="F87" s="1">
         <v>6.28E-10</v>
       </c>
       <c r="G87">
@@ -7463,7 +7462,7 @@
       <c r="I87">
         <v>296</v>
       </c>
-      <c r="J87" s="2">
+      <c r="J87" s="1">
         <v>3.2299999999999998E-9</v>
       </c>
       <c r="K87">
@@ -7485,7 +7484,7 @@
         <v>21.7</v>
       </c>
       <c r="Q87">
-        <v>0.13700000000000001</v>
+        <v>0.128</v>
       </c>
       <c r="R87">
         <v>3.27</v>
@@ -7507,7 +7506,7 @@
       <c r="B88" t="s">
         <v>281</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" t="s">
         <v>282</v>
       </c>
       <c r="D88">
@@ -7550,10 +7549,10 @@
         <v>21.7</v>
       </c>
       <c r="Q88">
-        <v>5.0200000000000002E-2</v>
-      </c>
-      <c r="R88">
-        <v>11.5</v>
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="R88" t="s">
+        <v>24</v>
       </c>
       <c r="S88" t="s">
         <v>24</v>
@@ -7572,7 +7571,7 @@
       <c r="B89" t="s">
         <v>284</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" t="s">
         <v>285</v>
       </c>
       <c r="D89">
@@ -7581,7 +7580,7 @@
       <c r="E89">
         <v>255</v>
       </c>
-      <c r="F89" s="2">
+      <c r="F89" s="1">
         <v>1.73E-10</v>
       </c>
       <c r="G89">
@@ -7593,7 +7592,7 @@
       <c r="I89">
         <v>129</v>
       </c>
-      <c r="J89" s="2">
+      <c r="J89" s="1">
         <v>4.01E-9</v>
       </c>
       <c r="K89">
@@ -7615,7 +7614,7 @@
         <v>6.25</v>
       </c>
       <c r="Q89">
-        <v>0.19400000000000001</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="R89">
         <v>5.77</v>
@@ -7637,7 +7636,7 @@
       <c r="B90" t="s">
         <v>287</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" t="s">
         <v>288</v>
       </c>
       <c r="D90">
@@ -7646,7 +7645,7 @@
       <c r="E90">
         <v>401</v>
       </c>
-      <c r="F90" s="2">
+      <c r="F90" s="1">
         <v>2.3899999999999999E-8</v>
       </c>
       <c r="G90">
@@ -7658,16 +7657,16 @@
       <c r="I90">
         <v>34.299999999999997</v>
       </c>
-      <c r="J90" s="2">
+      <c r="J90" s="1">
         <v>2.1900000000000001E-8</v>
       </c>
-      <c r="K90" s="2">
+      <c r="K90" s="1">
         <v>2.1299999999999999E-7</v>
       </c>
       <c r="L90">
         <v>68.400000000000006</v>
       </c>
-      <c r="M90" s="2">
+      <c r="M90" s="1">
         <v>1.89E-8</v>
       </c>
       <c r="N90">
@@ -7680,10 +7679,10 @@
         <v>21.7</v>
       </c>
       <c r="Q90">
-        <v>9.2599999999999996E-4</v>
-      </c>
-      <c r="R90">
-        <v>21.4</v>
+        <v>1.17E-3</v>
+      </c>
+      <c r="R90" t="s">
+        <v>24</v>
       </c>
       <c r="S90" t="s">
         <v>24</v>
@@ -7702,7 +7701,7 @@
       <c r="B91" t="s">
         <v>290</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" t="s">
         <v>291</v>
       </c>
       <c r="D91">
@@ -7711,7 +7710,7 @@
       <c r="E91">
         <v>335</v>
       </c>
-      <c r="F91" s="2">
+      <c r="F91" s="1">
         <v>7.4600000000000003E-9</v>
       </c>
       <c r="G91">
@@ -7723,7 +7722,7 @@
       <c r="I91">
         <v>160</v>
       </c>
-      <c r="J91" s="2">
+      <c r="J91" s="1">
         <v>1.5700000000000002E-8</v>
       </c>
       <c r="K91">
@@ -7745,7 +7744,7 @@
         <v>21.7</v>
       </c>
       <c r="Q91">
-        <v>0.182</v>
+        <v>0.106</v>
       </c>
       <c r="R91">
         <v>2.1</v>
@@ -7767,7 +7766,7 @@
       <c r="B92" t="s">
         <v>293</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" t="s">
         <v>294</v>
       </c>
       <c r="D92">
@@ -7776,7 +7775,7 @@
       <c r="E92">
         <v>347</v>
       </c>
-      <c r="F92" s="2">
+      <c r="F92" s="1">
         <v>1.3200000000000001E-5</v>
       </c>
       <c r="G92">
@@ -7788,7 +7787,7 @@
       <c r="I92">
         <v>52.8</v>
       </c>
-      <c r="J92" s="2">
+      <c r="J92" s="1">
         <v>1.1999999999999999E-6</v>
       </c>
       <c r="K92">
@@ -7798,7 +7797,7 @@
         <v>1.02</v>
       </c>
       <c r="M92">
-        <v>0.03</v>
+        <v>2.9600000000000001E-2</v>
       </c>
       <c r="N92">
         <v>6.84</v>
@@ -7810,10 +7809,10 @@
         <v>21.7</v>
       </c>
       <c r="Q92">
-        <v>3.8100000000000002E-2</v>
+        <v>3.9199999999999999E-2</v>
       </c>
       <c r="R92">
-        <v>2.0699999999999998</v>
+        <v>2.08</v>
       </c>
       <c r="S92">
         <v>2.64E-2</v>
@@ -7832,7 +7831,7 @@
       <c r="B93" t="s">
         <v>296</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" t="s">
         <v>297</v>
       </c>
       <c r="D93">
@@ -7871,14 +7870,14 @@
       <c r="O93">
         <v>0.73899999999999999</v>
       </c>
-      <c r="P93" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q93" t="s">
-        <v>24</v>
-      </c>
-      <c r="R93">
-        <v>12.2</v>
+      <c r="P93">
+        <v>21.7</v>
+      </c>
+      <c r="Q93">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="R93" t="s">
+        <v>24</v>
       </c>
       <c r="S93" t="s">
         <v>24</v>
@@ -7897,7 +7896,7 @@
       <c r="B94" t="s">
         <v>299</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" t="s">
         <v>300</v>
       </c>
       <c r="D94">
@@ -7906,7 +7905,7 @@
       <c r="E94">
         <v>220</v>
       </c>
-      <c r="F94" s="2">
+      <c r="F94" s="1">
         <v>9.7399999999999999E-8</v>
       </c>
       <c r="G94">
@@ -7962,7 +7961,7 @@
       <c r="B95" t="s">
         <v>302</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" t="s">
         <v>303</v>
       </c>
       <c r="D95">
@@ -7971,7 +7970,7 @@
       <c r="E95">
         <v>189</v>
       </c>
-      <c r="F95" s="2">
+      <c r="F95" s="1">
         <v>1.9200000000000001E-10</v>
       </c>
       <c r="G95">
@@ -7993,7 +7992,7 @@
         <v>1.64</v>
       </c>
       <c r="M95">
-        <v>5.0000000000000001E-3</v>
+        <v>4.7800000000000004E-3</v>
       </c>
       <c r="N95">
         <v>0</v>
@@ -8027,7 +8026,7 @@
       <c r="B96" t="s">
         <v>305</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" t="s">
         <v>306</v>
       </c>
       <c r="D96">
@@ -8036,7 +8035,7 @@
       <c r="E96">
         <v>332</v>
       </c>
-      <c r="F96" s="2">
+      <c r="F96" s="1">
         <v>4.9900000000000003E-10</v>
       </c>
       <c r="G96">
@@ -8048,7 +8047,7 @@
       <c r="I96">
         <v>248</v>
       </c>
-      <c r="J96" s="2">
+      <c r="J96" s="1">
         <v>1.1200000000000001E-6</v>
       </c>
       <c r="K96">
@@ -8070,7 +8069,7 @@
         <v>6.25</v>
       </c>
       <c r="Q96">
-        <v>6.6000000000000003E-2</v>
+        <v>8.4599999999999995E-2</v>
       </c>
       <c r="R96">
         <v>10.1</v>
@@ -8092,7 +8091,7 @@
       <c r="B97" t="s">
         <v>308</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" t="s">
         <v>309</v>
       </c>
       <c r="D97">
@@ -8101,7 +8100,7 @@
       <c r="E97">
         <v>365</v>
       </c>
-      <c r="F97" s="2">
+      <c r="F97" s="1">
         <v>5.9100000000000004E-7</v>
       </c>
       <c r="G97">
@@ -8113,17 +8112,17 @@
       <c r="I97">
         <v>101</v>
       </c>
-      <c r="J97" s="2">
+      <c r="J97" s="1">
         <v>1.6499999999999999E-8</v>
       </c>
-      <c r="K97" s="2">
+      <c r="K97" s="1">
         <v>2.03E-7</v>
       </c>
       <c r="L97">
         <v>18.5</v>
       </c>
-      <c r="M97">
-        <v>0</v>
+      <c r="M97" t="s">
+        <v>24</v>
       </c>
       <c r="N97">
         <v>47</v>
@@ -8135,7 +8134,7 @@
         <v>21.7</v>
       </c>
       <c r="Q97">
-        <v>1.03E-2</v>
+        <v>1.11E-2</v>
       </c>
       <c r="R97">
         <v>15.5</v>
@@ -8157,7 +8156,7 @@
       <c r="B98" t="s">
         <v>311</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" t="s">
         <v>312</v>
       </c>
       <c r="D98">
@@ -8166,7 +8165,7 @@
       <c r="E98">
         <v>315</v>
       </c>
-      <c r="F98" s="2">
+      <c r="F98" s="1">
         <v>1.3799999999999999E-8</v>
       </c>
       <c r="G98">
@@ -8178,7 +8177,7 @@
       <c r="I98">
         <v>145</v>
       </c>
-      <c r="J98" s="2">
+      <c r="J98" s="1">
         <v>1.3599999999999999E-6</v>
       </c>
       <c r="K98">
@@ -8200,7 +8199,7 @@
         <v>21.7</v>
       </c>
       <c r="Q98">
-        <v>0.374</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="R98">
         <v>21.1</v>
@@ -8222,7 +8221,7 @@
       <c r="B99" t="s">
         <v>314</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" t="s">
         <v>315</v>
       </c>
       <c r="D99">
@@ -8231,7 +8230,7 @@
       <c r="E99">
         <v>115</v>
       </c>
-      <c r="F99" s="2">
+      <c r="F99" s="1">
         <v>1.1E-5</v>
       </c>
       <c r="G99">
@@ -8287,7 +8286,7 @@
       <c r="B100" t="s">
         <v>317</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" t="s">
         <v>318</v>
       </c>
       <c r="D100">
@@ -8296,7 +8295,7 @@
       <c r="E100">
         <v>263</v>
       </c>
-      <c r="F100" s="2">
+      <c r="F100" s="1">
         <v>6.4099999999999998E-7</v>
       </c>
       <c r="G100">
@@ -8352,7 +8351,7 @@
       <c r="B101" t="s">
         <v>320</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" t="s">
         <v>321</v>
       </c>
       <c r="D101">
@@ -8361,7 +8360,7 @@
       <c r="E101">
         <v>79.099999999999994</v>
       </c>
-      <c r="F101" s="2">
+      <c r="F101" s="1">
         <v>9.3599999999999998E-5</v>
       </c>
       <c r="G101">
@@ -8397,8 +8396,8 @@
       <c r="Q101" t="s">
         <v>24</v>
       </c>
-      <c r="R101">
-        <v>8.31</v>
+      <c r="R101" t="s">
+        <v>24</v>
       </c>
       <c r="S101" t="s">
         <v>24</v>
@@ -8417,7 +8416,7 @@
       <c r="B102" t="s">
         <v>323</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" t="s">
         <v>324</v>
       </c>
       <c r="D102">
@@ -8426,7 +8425,7 @@
       <c r="E102">
         <v>385</v>
       </c>
-      <c r="F102" s="2">
+      <c r="F102" s="1">
         <v>1.57E-6</v>
       </c>
       <c r="G102">
@@ -8438,17 +8437,17 @@
       <c r="I102">
         <v>34.4</v>
       </c>
-      <c r="J102" s="2">
+      <c r="J102" s="1">
         <v>8.0200000000000001E-7</v>
       </c>
-      <c r="K102" s="2">
+      <c r="K102" s="1">
         <v>6.3100000000000002E-5</v>
       </c>
       <c r="L102">
         <v>250</v>
       </c>
       <c r="M102">
-        <v>6.0000000000000001E-3</v>
+        <v>6.0800000000000003E-3</v>
       </c>
       <c r="N102">
         <v>86.9</v>
@@ -8460,7 +8459,7 @@
         <v>21.7</v>
       </c>
       <c r="Q102">
-        <v>1.03E-2</v>
+        <v>1.01E-2</v>
       </c>
       <c r="R102">
         <v>9.11</v>

</xml_diff>